<commit_message>
Update with new publications from 2025
</commit_message>
<xml_diff>
--- a/static/publications/publications.xlsx
+++ b/static/publications/publications.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dezerae\Documents\Current Writing\240101_MSC015_Operation-Lab-Launch\website\thenervlab.org\static\publications\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66154837-A0A7-4F01-9D21-C4A1B6DEB4F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF1E318-8C4C-44B4-A89D-E238C4620E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="189">
   <si>
     <t>Title</t>
   </si>
@@ -379,9 +379,6 @@
     <t>Single-molecule observations of human small heat shock proteins in complex with aggregation-prone client proteins</t>
   </si>
   <si>
-    <t>Rice L, Marzano N, Cox D, van Oijen A, Ecroyd H</t>
-  </si>
-  <si>
     <t>Rice L</t>
   </si>
   <si>
@@ -424,9 +421,6 @@
     <t>https://doi.org/10.5281/zenodo.10684022</t>
   </si>
   <si>
-    <t>Fingerprinting disease-derived protein aggregates reveals unique signature of Motor Neuron Disease</t>
-  </si>
-  <si>
     <t>Cox D, Burke M, Milani S, White MA, Waldron FM, Böken D, Lobanova E, Sreedharan J, Gregory JM, Klenerman D.</t>
   </si>
   <si>
@@ -521,6 +515,78 @@
   </si>
   <si>
     <t>tdp-simpull</t>
+  </si>
+  <si>
+    <t>Advanced Science</t>
+  </si>
+  <si>
+    <t>Biochemical Journal</t>
+  </si>
+  <si>
+    <t>10.1042/BCJ20240473</t>
+  </si>
+  <si>
+    <t>10.1002/advs.202505484</t>
+  </si>
+  <si>
+    <t>Quantitative Profiling of Nanoscopic Protein Aggregates Reveals Specific Fingerprint of TDP-43-Positive Assemblies in Motor Neuron Disease</t>
+  </si>
+  <si>
+    <t>Small tau aggregates exhibit disease-specific molecular profiles across tauopathies</t>
+  </si>
+  <si>
+    <t>Rice L, Marzano N, Cox D, Skewes B, van Oijen A, Ecroyd H</t>
+  </si>
+  <si>
+    <t>Böken D, Huang M, Wu Y, Fertan E, Lam JYL, Meisl G, Baig S, Rowe JB, Smith C, Quaegebeur A, Cox D, McEwan WA, Klenerman D.</t>
+  </si>
+  <si>
+    <t>bioRxiv</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1101/2025.06.10.658934</t>
+  </si>
+  <si>
+    <t>Direct single-molecule visualization of Hsp90-mediated relief of a Hsp70-folding block</t>
+  </si>
+  <si>
+    <t>Marzano NR, Skewes B, McMahon S, Rice L, Cox D, van Oijen AM, Ecroyd H.</t>
+  </si>
+  <si>
+    <t>Marzano NR</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1101/2025.08.25.672245</t>
+  </si>
+  <si>
+    <t>Differential inclusion formation of an aggregation-prone protein reveals differences in the proteostasis capacity of neuronal cell lines</t>
+  </si>
+  <si>
+    <t>McMahon S, Cox D, Cheng F, Lee A, Yerbury JJ, Ecroyd H.</t>
+  </si>
+  <si>
+    <t>McMahon S</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1101/2025.08.26.672484</t>
+  </si>
+  <si>
+    <t>tau-omics</t>
+  </si>
+  <si>
+    <t>chaperone-moa</t>
+  </si>
+  <si>
+    <t>neuronal-proteostasis</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.5281/zenodo.15635269</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.5281/zenodo.16791519</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.5281/zenodo.16892326</t>
   </si>
 </sst>
 </file>
@@ -1004,8 +1070,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1381,19 +1451,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="84.85546875" style="1" customWidth="1"/>
+    <col min="2" max="11" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -1424,11 +1496,11 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>110</v>
       </c>
       <c r="B2" t="s">
@@ -1447,11 +1519,11 @@
         <v>113</v>
       </c>
       <c r="K2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>114</v>
       </c>
       <c r="B3" t="s">
@@ -1470,11 +1542,11 @@
         <v>117</v>
       </c>
       <c r="K3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>107</v>
       </c>
       <c r="B4" t="s">
@@ -1493,11 +1565,11 @@
         <v>109</v>
       </c>
       <c r="K4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>103</v>
       </c>
       <c r="B5" t="s">
@@ -1516,11 +1588,11 @@
         <v>106</v>
       </c>
       <c r="K5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B6" t="s">
@@ -1539,11 +1611,11 @@
         <v>98</v>
       </c>
       <c r="K6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B7" t="s">
@@ -1562,11 +1634,11 @@
         <v>91</v>
       </c>
       <c r="K7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B8" t="s">
@@ -1585,11 +1657,11 @@
         <v>102</v>
       </c>
       <c r="K8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B9" t="s">
@@ -1608,11 +1680,11 @@
         <v>95</v>
       </c>
       <c r="K9" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B10" t="s">
@@ -1634,11 +1706,11 @@
         <v>68</v>
       </c>
       <c r="K10" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B11" t="s">
@@ -1657,11 +1729,11 @@
         <v>82</v>
       </c>
       <c r="K11" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B12" t="s">
@@ -1680,11 +1752,11 @@
         <v>73</v>
       </c>
       <c r="K12" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B13" t="s">
@@ -1703,11 +1775,11 @@
         <v>77</v>
       </c>
       <c r="K13" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B14" t="s">
@@ -1729,11 +1801,11 @@
         <v>87</v>
       </c>
       <c r="K14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B15" t="s">
@@ -1752,11 +1824,11 @@
         <v>62</v>
       </c>
       <c r="K15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B16" t="s">
@@ -1781,11 +1853,11 @@
         <v>29</v>
       </c>
       <c r="K16" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B17" t="s">
@@ -1810,11 +1882,11 @@
         <v>22</v>
       </c>
       <c r="K17" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B18" t="s">
@@ -1839,11 +1911,11 @@
         <v>48</v>
       </c>
       <c r="K18" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B19" t="s">
@@ -1865,11 +1937,11 @@
         <v>42</v>
       </c>
       <c r="K19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B20" t="s">
@@ -1894,11 +1966,11 @@
         <v>36</v>
       </c>
       <c r="K20" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B21" t="s">
@@ -1917,11 +1989,11 @@
         <v>53</v>
       </c>
       <c r="K21" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B22" t="s">
@@ -1940,35 +2012,35 @@
         <v>57</v>
       </c>
       <c r="K22" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B23" t="s">
         <v>125</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>126</v>
       </c>
-      <c r="C23" t="s">
-        <v>127</v>
-      </c>
       <c r="D23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E23">
         <v>2023</v>
       </c>
       <c r="G23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K23" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>162</v>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>160</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
@@ -1992,91 +2064,175 @@
         <v>15</v>
       </c>
       <c r="K24" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B25" t="s">
         <v>129</v>
-      </c>
-      <c r="B25" t="s">
-        <v>130</v>
       </c>
       <c r="C25" t="s">
         <v>18</v>
       </c>
       <c r="D25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E25">
         <v>2024</v>
       </c>
       <c r="F25" t="s">
+        <v>131</v>
+      </c>
+      <c r="I25" t="s">
         <v>132</v>
       </c>
-      <c r="I25" t="s">
+      <c r="K25" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B26" t="s">
+        <v>171</v>
+      </c>
+      <c r="C26" t="s">
+        <v>119</v>
+      </c>
+      <c r="D26" t="s">
+        <v>166</v>
+      </c>
+      <c r="E26">
+        <v>2025</v>
+      </c>
+      <c r="F26" t="s">
+        <v>167</v>
+      </c>
+      <c r="G26" t="s">
+        <v>121</v>
+      </c>
+      <c r="H26" t="s">
+        <v>122</v>
+      </c>
+      <c r="I26" t="s">
+        <v>123</v>
+      </c>
+      <c r="K26" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B27" t="s">
         <v>133</v>
-      </c>
-      <c r="K25" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>118</v>
-      </c>
-      <c r="B26" t="s">
-        <v>119</v>
-      </c>
-      <c r="C26" t="s">
-        <v>120</v>
-      </c>
-      <c r="D26" t="s">
-        <v>121</v>
-      </c>
-      <c r="E26">
-        <v>2024</v>
-      </c>
-      <c r="G26" t="s">
-        <v>122</v>
-      </c>
-      <c r="H26" t="s">
-        <v>123</v>
-      </c>
-      <c r="I26" t="s">
-        <v>124</v>
-      </c>
-      <c r="K26" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>134</v>
-      </c>
-      <c r="B27" t="s">
-        <v>135</v>
       </c>
       <c r="C27" t="s">
         <v>18</v>
       </c>
       <c r="D27" t="s">
-        <v>121</v>
+        <v>165</v>
       </c>
       <c r="E27">
         <v>2025</v>
       </c>
+      <c r="F27" t="s">
+        <v>168</v>
+      </c>
       <c r="G27" t="s">
+        <v>134</v>
+      </c>
+      <c r="H27" t="s">
+        <v>135</v>
+      </c>
+      <c r="I27" t="s">
         <v>136</v>
       </c>
-      <c r="H27" t="s">
-        <v>137</v>
-      </c>
-      <c r="I27" t="s">
-        <v>138</v>
-      </c>
       <c r="K27" t="s">
-        <v>166</v>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B28" t="s">
+        <v>172</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" t="s">
+        <v>173</v>
+      </c>
+      <c r="E28">
+        <v>2025</v>
+      </c>
+      <c r="G28" t="s">
+        <v>174</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="K28" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B29" t="s">
+        <v>176</v>
+      </c>
+      <c r="C29" t="s">
+        <v>177</v>
+      </c>
+      <c r="D29" t="s">
+        <v>173</v>
+      </c>
+      <c r="E29">
+        <v>2025</v>
+      </c>
+      <c r="G29" t="s">
+        <v>178</v>
+      </c>
+      <c r="I29" t="s">
+        <v>187</v>
+      </c>
+      <c r="K29" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B30" t="s">
+        <v>180</v>
+      </c>
+      <c r="C30" t="s">
+        <v>181</v>
+      </c>
+      <c r="D30" t="s">
+        <v>173</v>
+      </c>
+      <c r="E30">
+        <v>2025</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="K30" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>